<commit_message>
tambah analisa data lulusan S2 jenis kelamin
</commit_message>
<xml_diff>
--- a/analisa jml_mhs_lulus_s1.xlsx
+++ b/analisa jml_mhs_lulus_s1.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="mhs_lulus_s1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="mhs_lulus_s2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="76">
   <si>
     <t>Fisika S1</t>
   </si>
@@ -166,6 +166,93 @@
   </si>
   <si>
     <t>group by substring(a_mhs.NRP, 1,2)+substring(a_mhs.NRP, 5,3), substring(mhs.NRP, 1,2)+substring(mhs.NRP, 5,3), mhs.SEX, prodi.NAMAPROGRAM</t>
+  </si>
+  <si>
+    <t>Fisika S2</t>
+  </si>
+  <si>
+    <t>Matematika S2</t>
+  </si>
+  <si>
+    <t>Statistika S2</t>
+  </si>
+  <si>
+    <t>Kimia S2</t>
+  </si>
+  <si>
+    <t>T. Mesin S2</t>
+  </si>
+  <si>
+    <t>T. Fisika S2</t>
+  </si>
+  <si>
+    <t>S2 T Material dan Metalurgi</t>
+  </si>
+  <si>
+    <t>Arsitektur S2 Pemukim. Kota</t>
+  </si>
+  <si>
+    <t>T. Geomatika S2</t>
+  </si>
+  <si>
+    <t>T. Perkapalan S2 Trans. Kelaut</t>
+  </si>
+  <si>
+    <t>T. Informatika S2</t>
+  </si>
+  <si>
+    <t>MMT S2 Manaj. Industri</t>
+  </si>
+  <si>
+    <t>T. Elektro S2</t>
+  </si>
+  <si>
+    <t>T. Kimia S2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T. Sipil S2 </t>
+  </si>
+  <si>
+    <t>T. Sipil S2</t>
+  </si>
+  <si>
+    <t>Jumlah Lulusan S2- Mudji Sukur</t>
+  </si>
+  <si>
+    <t>T. Lingkungan S2</t>
+  </si>
+  <si>
+    <t>Arsitektur S2</t>
+  </si>
+  <si>
+    <t>T. Industri</t>
+  </si>
+  <si>
+    <t>T. Industr</t>
+  </si>
+  <si>
+    <t>Seliish</t>
+  </si>
+  <si>
+    <t>Mudji Sukur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from dbo.MAHASISWA mhs, dbo.AKTIVITASMHS a_mhs, dbo.PROGRAMSTUDI prodi </t>
+  </si>
+  <si>
+    <t>where a_mhs.NRP = mhs.NRP and substring(a_mhs.NRP, 7,1) != '0' and substring(mhs.NRP, 7,1) != '0'</t>
+  </si>
+  <si>
+    <t>and substring(a_mhs.NRP,5,1) = '2' and substring(mhs.NRP,5,1) = '2' and a_mhs.PERIODESEM in ('20142','20151') and a_mhs.STATUSMAHASISWA = 'L'</t>
+  </si>
+  <si>
+    <t>Data_its</t>
+  </si>
+  <si>
+    <t>where t.Kode_jenjang_pendidikan = '1' and t.tahun_pelaporan = '2015'</t>
+  </si>
+  <si>
+    <t>Jumlah Lulusan S2- Data its</t>
   </si>
 </sst>
 </file>
@@ -188,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +286,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
       </patternFill>
     </fill>
   </fills>
@@ -291,11 +383,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -306,9 +399,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -589,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50:G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,12 +1732,837 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>11201</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1">
+        <v>27</v>
+      </c>
+      <c r="F2" s="8">
+        <f>D2-E2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>11201</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1">
+        <v>30</v>
+      </c>
+      <c r="F3" s="8">
+        <f t="shared" ref="F3:F35" si="0">D3-E3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>12201</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1">
+        <v>24</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>12201</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1">
+        <v>28</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>13201</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1">
+        <v>30</v>
+      </c>
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>13201</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>56</v>
+      </c>
+      <c r="E7" s="1">
+        <v>56</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>14201</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1">
+        <v>19</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>14201</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1">
+        <v>38</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>21201</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1">
+        <v>37</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>21201</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1">
+        <v>17</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>22201</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>84</v>
+      </c>
+      <c r="E12" s="1">
+        <v>84</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>22201</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>51</v>
+      </c>
+      <c r="E13" s="1">
+        <v>51</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>23201</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1">
+        <v>11</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>23201</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>16</v>
+      </c>
+      <c r="E15" s="1">
+        <v>16</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>24201</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1">
+        <v>11</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>24201</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1">
+        <v>6</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>25201</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1">
+        <v>14</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>25201</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>37</v>
+      </c>
+      <c r="E19" s="1">
+        <v>37</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>27201</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>14</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>27201</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4</v>
+      </c>
+      <c r="E21" s="14">
+        <v>0</v>
+      </c>
+      <c r="F21" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>31201</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>53</v>
+      </c>
+      <c r="E22" s="1">
+        <v>53</v>
+      </c>
+      <c r="F22" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>31201</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>32</v>
+      </c>
+      <c r="E23" s="1">
+        <v>32</v>
+      </c>
+      <c r="F23" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>32201</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>23</v>
+      </c>
+      <c r="E24" s="1">
+        <v>24</v>
+      </c>
+      <c r="F24" s="8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>32201</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>50</v>
+      </c>
+      <c r="E25" s="1">
+        <v>49</v>
+      </c>
+      <c r="F25" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>33201</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1">
+        <v>17</v>
+      </c>
+      <c r="F26" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>33201</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>32</v>
+      </c>
+      <c r="E27" s="1">
+        <v>32</v>
+      </c>
+      <c r="F27" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>35201</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1">
+        <v>7</v>
+      </c>
+      <c r="F28" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>35201</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>12</v>
+      </c>
+      <c r="E29" s="1">
+        <v>12</v>
+      </c>
+      <c r="F29" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>41202</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>29</v>
+      </c>
+      <c r="E30" s="1">
+        <v>29</v>
+      </c>
+      <c r="F30" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>41202</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>5</v>
+      </c>
+      <c r="E31" s="1">
+        <v>5</v>
+      </c>
+      <c r="F31" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>51201</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>47</v>
+      </c>
+      <c r="E32" s="1">
+        <v>47</v>
+      </c>
+      <c r="F32" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>51201</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>27</v>
+      </c>
+      <c r="E33" s="1">
+        <v>27</v>
+      </c>
+      <c r="F33" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>91201</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>90</v>
+      </c>
+      <c r="E34" s="1">
+        <v>90</v>
+      </c>
+      <c r="F34" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>91201</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2">
+        <v>33</v>
+      </c>
+      <c r="E35" s="2">
+        <v>33</v>
+      </c>
+      <c r="F35" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>